<commit_message>
Improved French sentiment analysis and fixed UI issues
</commit_message>
<xml_diff>
--- a/uploads/pj.xlsx
+++ b/uploads/pj.xlsx
@@ -459,9 +459,6 @@
     <t>Audit SM</t>
   </si>
   <si>
-    <t>Industrie Automobile</t>
-  </si>
-  <si>
     <t>Mohamed Amine SOUID - asouid@kpmg.com</t>
   </si>
   <si>
@@ -571,6 +568,9 @@
   </si>
   <si>
     <t>1226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industrie </t>
   </si>
 </sst>
 </file>
@@ -914,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1106,7 +1106,7 @@
         <v>25</v>
       </c>
       <c r="W2">
-        <v>0.28999999999999998</v>
+        <v>33</v>
       </c>
       <c r="X2">
         <v>-5.85</v>
@@ -1195,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X3">
         <v>0</v>
@@ -1266,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -1352,7 +1352,7 @@
         <v>15</v>
       </c>
       <c r="W5">
-        <v>2.95</v>
+        <v>10</v>
       </c>
       <c r="X5">
         <v>0.83</v>
@@ -1438,7 +1438,7 @@
         <v>147</v>
       </c>
       <c r="W6">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="X6">
         <v>-5.75</v>
@@ -1521,7 +1521,7 @@
         <v>4</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="X7">
         <v>0</v>
@@ -1607,7 +1607,7 @@
         <v>23</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="X8">
         <v>0</v>
@@ -1696,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="X9">
         <v>0</v>
@@ -1734,7 +1734,7 @@
         <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H10" t="s">
         <v>43</v>
@@ -1779,7 +1779,7 @@
         <v>15</v>
       </c>
       <c r="W10">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="X10">
         <v>0.87</v>
@@ -1862,7 +1862,7 @@
         <v>27</v>
       </c>
       <c r="W11">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="X11">
         <v>0.78</v>
@@ -1960,13 +1960,13 @@
         <v>14</v>
       </c>
       <c r="W12">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="X12">
         <v>0.83</v>
       </c>
       <c r="Y12" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="AI12" t="s">
         <v>127</v>
@@ -2046,7 +2046,7 @@
         <v>158.5</v>
       </c>
       <c r="W13">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="X13">
         <v>0</v>
@@ -2132,7 +2132,7 @@
         <v>110</v>
       </c>
       <c r="W14">
-        <v>1.83</v>
+        <v>23</v>
       </c>
       <c r="X14">
         <v>0.56000000000000005</v>
@@ -2170,7 +2170,7 @@
         <v>140</v>
       </c>
       <c r="F15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H15" t="s">
         <v>43</v>
@@ -2209,7 +2209,7 @@
         <v>22</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X15">
         <v>0</v>
@@ -2247,7 +2247,7 @@
         <v>104</v>
       </c>
       <c r="F16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H16" t="s">
         <v>43</v>
@@ -2292,34 +2292,34 @@
         <v>18</v>
       </c>
       <c r="W16">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="X16">
         <v>0</v>
       </c>
       <c r="Y16" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z16" t="s">
         <v>146</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>147</v>
       </c>
       <c r="AI16" t="s">
         <v>143</v>
       </c>
       <c r="AJ16" t="s">
+        <v>147</v>
+      </c>
+      <c r="AK16" t="s">
         <v>148</v>
       </c>
-      <c r="AK16" t="s">
+      <c r="AL16" t="s">
+        <v>147</v>
+      </c>
+      <c r="AM16" t="s">
         <v>149</v>
       </c>
-      <c r="AL16" t="s">
-        <v>148</v>
-      </c>
-      <c r="AM16" t="s">
+      <c r="AN16" t="s">
         <v>150</v>
-      </c>
-      <c r="AN16" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.3">
@@ -2327,10 +2327,10 @@
         <v>61</v>
       </c>
       <c r="C17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" t="s">
         <v>152</v>
-      </c>
-      <c r="D17" t="s">
-        <v>153</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
@@ -2342,16 +2342,16 @@
         <v>45</v>
       </c>
       <c r="J17" t="s">
+        <v>153</v>
+      </c>
+      <c r="K17" t="s">
+        <v>46</v>
+      </c>
+      <c r="L17" t="s">
         <v>154</v>
       </c>
-      <c r="K17" t="s">
-        <v>46</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>155</v>
-      </c>
-      <c r="M17" t="s">
-        <v>156</v>
       </c>
       <c r="N17" t="s">
         <v>86</v>
@@ -2363,7 +2363,7 @@
         <v>49</v>
       </c>
       <c r="Q17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R17">
         <v>40</v>
@@ -2381,31 +2381,31 @@
         <v>31</v>
       </c>
       <c r="W17">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="X17">
         <v>0</v>
       </c>
       <c r="Y17" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="AI17" t="s">
+        <v>157</v>
+      </c>
+      <c r="AJ17" t="s">
         <v>158</v>
       </c>
-      <c r="AJ17" t="s">
+      <c r="AK17" t="s">
+        <v>157</v>
+      </c>
+      <c r="AL17" t="s">
         <v>159</v>
       </c>
-      <c r="AK17" t="s">
+      <c r="AM17" t="s">
         <v>158</v>
       </c>
-      <c r="AL17" t="s">
-        <v>160</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>159</v>
-      </c>
       <c r="AN17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.3">
@@ -2413,31 +2413,31 @@
         <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D18" t="s">
         <v>104</v>
       </c>
       <c r="F18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H18" t="s">
         <v>60</v>
       </c>
       <c r="I18" t="s">
+        <v>162</v>
+      </c>
+      <c r="J18" t="s">
         <v>163</v>
       </c>
-      <c r="J18" t="s">
-        <v>164</v>
-      </c>
       <c r="K18" t="s">
         <v>46</v>
       </c>
       <c r="L18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N18" t="s">
         <v>71</v>
@@ -2458,28 +2458,28 @@
         <v>13.3</v>
       </c>
       <c r="W18">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="X18">
         <v>0</v>
       </c>
       <c r="Y18" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="AI18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AJ18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AK18" t="s">
         <v>81</v>
       </c>
       <c r="AL18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AM18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AN18" t="s">
         <v>81</v>
@@ -2490,22 +2490,22 @@
         <v>67</v>
       </c>
       <c r="C19" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" t="s">
         <v>166</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>167</v>
-      </c>
-      <c r="F19" t="s">
-        <v>168</v>
       </c>
       <c r="H19" t="s">
         <v>43</v>
       </c>
       <c r="I19" t="s">
+        <v>168</v>
+      </c>
+      <c r="J19" t="s">
         <v>169</v>
-      </c>
-      <c r="J19" t="s">
-        <v>170</v>
       </c>
       <c r="K19" t="s">
         <v>46</v>
@@ -2520,7 +2520,7 @@
         <v>71</v>
       </c>
       <c r="Q19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R19">
         <v>0</v>
@@ -2535,31 +2535,31 @@
         <v>37</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="X19">
         <v>0</v>
       </c>
       <c r="Y19" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="AI19" t="s">
+        <v>171</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>171</v>
+      </c>
+      <c r="AK19" t="s">
         <v>172</v>
       </c>
-      <c r="AJ19" t="s">
-        <v>172</v>
-      </c>
-      <c r="AK19" t="s">
+      <c r="AL19" t="s">
+        <v>171</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>171</v>
+      </c>
+      <c r="AN19" t="s">
         <v>173</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>172</v>
-      </c>
-      <c r="AM19" t="s">
-        <v>172</v>
-      </c>
-      <c r="AN19" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.3">
@@ -2567,7 +2567,7 @@
         <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D20" t="s">
         <v>104</v>
@@ -2576,25 +2576,25 @@
         <v>105</v>
       </c>
       <c r="G20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H20" t="s">
         <v>43</v>
       </c>
       <c r="I20" t="s">
+        <v>176</v>
+      </c>
+      <c r="J20" t="s">
         <v>177</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" t="s">
         <v>178</v>
       </c>
-      <c r="K20" t="s">
-        <v>46</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>179</v>
-      </c>
-      <c r="M20" t="s">
-        <v>180</v>
       </c>
       <c r="N20" t="s">
         <v>48</v>
@@ -2606,7 +2606,7 @@
         <v>49</v>
       </c>
       <c r="Q20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="R20">
         <v>1100</v>
@@ -2624,34 +2624,34 @@
         <v>13</v>
       </c>
       <c r="W20">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="X20">
         <v>0</v>
       </c>
       <c r="Y20" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="Z20" t="s">
+        <v>181</v>
+      </c>
+      <c r="AI20" t="s">
         <v>182</v>
       </c>
-      <c r="AI20" t="s">
-        <v>183</v>
-      </c>
       <c r="AJ20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AL20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AM20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AN20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>